<commit_message>
Finished assembling materials for W2S2.
</commit_message>
<xml_diff>
--- a/Names_list.xlsx
+++ b/Names_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/matthieu_demari_sutd_edu_sg/Documents/Teaching folder for web/9. DL @ SUTD 2021-ongoing/Teaching Materials/1. Lectures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED74EDAE-DCC8-4190-A08F-B1CAE85CFE09}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8609FA23-6578-43B2-AF05-8AE5216620AC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1185" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Family name</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>Patrick</t>
+  </si>
+  <si>
+    <t>Hazan</t>
+  </si>
+  <si>
+    <t>Elad</t>
+  </si>
+  <si>
+    <t>Kingma</t>
+  </si>
+  <si>
+    <t>Ba</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
   </si>
 </sst>
 </file>
@@ -149,6 +164,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,6 +581,45 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>